<commit_message>
feat!: new sheet CONDUCTOR_operation in file conductor_definition
Define sheet CONDUCTOR_operation to manage the electric module.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA75F3D-9969-40AD-815B-774C6C7B0013}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{461CCD28-8686-4077-910C-0BE7A8665E5C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
     <sheet name="CONDUCTOR_input" sheetId="10" r:id="rId2"/>
-    <sheet name="CONDUCTOR_COUPLING" sheetId="8" r:id="rId3"/>
+    <sheet name="CONDUCTOR_operation" sheetId="11" r:id="rId3"/>
+    <sheet name="CONDUCTOR_COUPLING" sheetId="8" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>XLENGTH</t>
   </si>
@@ -251,13 +252,46 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>EQUIPOTENTIAL_SURFACE_FLAG</t>
+  </si>
+  <si>
+    <t>Flag to define if there are equipotential surfaces. Possible values: TRUE = there are equipotential surfaces; FALSE = there are not equipotential surfaces. Defaults to TRUE</t>
+  </si>
+  <si>
+    <t>EQUIPOTENTIAL_SURFACE_NUMBER</t>
+  </si>
+  <si>
+    <t>The number of equipotential surfaces if EQUIPOTENTIAL_SURFACE_FLAG is true.</t>
+  </si>
+  <si>
+    <t>EQUIPOTENTIAL_SURFACE_COORDINATE</t>
+  </si>
+  <si>
+    <t>List of axial coordinates of the equipotential surfaces (cross section), separated by a comma. Ex, if at z = 0.5m z = 1.0m and z = 1.5m there are equipotential surfaces, write 0.5,1.0,1.5.</t>
+  </si>
+  <si>
+    <t>0.0,5.0,10.0</t>
+  </si>
+  <si>
+    <t>MAXIMUM_ITERATION_NUMBER</t>
+  </si>
+  <si>
+    <t>Maximum number of iteration allowed for iterative methods in the electric module.</t>
+  </si>
+  <si>
+    <t>INDUCTANCE_MODE</t>
+  </si>
+  <si>
+    <t>flag to select the method to evaluate the inductance. Possible values: 0 = iterative; 1 = analytical. Defaults to 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +310,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +451,37 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,24 +826,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="8"/>
+    <col min="6" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -785,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="1"/>
       <c r="D2" s="20"/>
@@ -794,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -816,7 +887,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -830,7 +901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -845,7 +916,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -860,7 +931,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>24</v>
       </c>
@@ -875,7 +946,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
@@ -890,7 +961,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
@@ -905,7 +976,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
@@ -920,7 +991,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
@@ -935,7 +1006,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -950,7 +1021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
@@ -965,7 +1036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>39</v>
       </c>
@@ -980,7 +1051,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>47</v>
       </c>
@@ -1012,20 +1083,20 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
@@ -1039,13 +1110,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="19">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1067,7 +1138,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>56</v>
       </c>
@@ -1101,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>58</v>
       </c>
@@ -1118,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>61</v>
       </c>
@@ -1135,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>62</v>
       </c>
@@ -1152,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
@@ -1186,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1201,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
@@ -1216,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1233,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
@@ -1250,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>12</v>
       </c>
@@ -1284,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>18</v>
       </c>
@@ -1318,7 +1389,7 @@
         <v>10001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>42</v>
       </c>
@@ -1335,7 +1406,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>41</v>
       </c>
@@ -1352,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>45</v>
       </c>
@@ -1370,7 +1441,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -1387,7 +1458,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>52</v>
       </c>
@@ -1404,7 +1475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>53</v>
       </c>
@@ -1429,6 +1500,156 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="str">
+        <f>CONDUCTOR_files!A1</f>
+        <v>CONDUCTOR</v>
+      </c>
+      <c r="B1" s="32">
+        <f>SUM(E2:AE2)</f>
+        <v>1</v>
+      </c>
+      <c r="E1" s="33">
+        <f>CONDUCTOR_files!E1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="33">
+        <f>IF(E$1 &gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="str">
+        <f>CONDUCTOR_files!A$3</f>
+        <v>Variable name</v>
+      </c>
+      <c r="B3" s="32" t="str">
+        <f>CONDUCTOR_files!B$3</f>
+        <v>Unit</v>
+      </c>
+      <c r="C3" s="32" t="str">
+        <f>CONDUCTOR_files!C$3</f>
+        <v>Variable type</v>
+      </c>
+      <c r="D3" s="32" t="str">
+        <f>CONDUCTOR_files!D$3</f>
+        <v>Note/comments</v>
+      </c>
+      <c r="E3" s="32" t="str">
+        <f>CONDUCTOR_files!E3</f>
+        <v>CONDUCTOR_1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="39">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="35">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1436,20 +1657,20 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="29" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>

</xml_diff>

<commit_message>
fix!: rename sheet CONDUCTOR_COUPLING.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{461CCD28-8686-4077-910C-0BE7A8665E5C}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E6628D5-1AF4-41F1-8179-DB83140FF348}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
     <sheet name="CONDUCTOR_input" sheetId="10" r:id="rId2"/>
     <sheet name="CONDUCTOR_operation" sheetId="11" r:id="rId3"/>
-    <sheet name="CONDUCTOR_COUPLING" sheetId="8" r:id="rId4"/>
+    <sheet name="CONDUCTOR_coupling" sheetId="8" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -1503,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1653,7 +1653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat!: update sheet CONDUCTOR_input of file conductor_definition.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E6628D5-1AF4-41F1-8179-DB83140FF348}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB2B835-C2ED-4653-9C41-68DB766D52D5}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
   <si>
     <t>XLENGTH</t>
   </si>
@@ -53,18 +53,12 @@
     <t>A</t>
   </si>
   <si>
-    <t>IOPFUN</t>
-  </si>
-  <si>
     <t>flag</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>TAUDUM</t>
-  </si>
-  <si>
     <t>STRUCTURE_ELEMENTS</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>IOP0_TOT</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t>EXTERNAL_FLOW</t>
   </si>
   <si>
-    <t>TAUDET</t>
-  </si>
-  <si>
     <t>XJBEG</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>Length of the conductor</t>
   </si>
   <si>
-    <t>current flag: 0 = constant; 1 = exponential decay from taudet to taudum; -1 = read from file; -2 = external function for current and its derivative after taudum</t>
-  </si>
-  <si>
     <t>transport current at time = 0;</t>
   </si>
   <si>
@@ -285,13 +270,37 @@
   </si>
   <si>
     <t>flag to select the method to evaluate the inductance. Possible values: 0 = iterative; 1 = analytical. Defaults to 0</t>
+  </si>
+  <si>
+    <t>I0_OP_MODE</t>
+  </si>
+  <si>
+    <t>I0_OP_TOT</t>
+  </si>
+  <si>
+    <t>current flag: 0 = constant; -1 = read from file; -2 = external function for current and its derivative after taudum</t>
+  </si>
+  <si>
+    <t>ELECTRIC_METHOD</t>
+  </si>
+  <si>
+    <t>flag to define the electric solution method: BE = Backward Euler; CN = Crank Nicholson</t>
+  </si>
+  <si>
+    <t>ELECTRIC_TIME_STEP</t>
+  </si>
+  <si>
+    <t>time step value for the electric transient solution. If None, uses the default value of dt/500 with dt the thermal time step.</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,13 +312,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,10 +370,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -467,20 +465,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,24 +832,24 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="9">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
@@ -857,215 +859,215 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
+      <c r="A2" s="12"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="10">
+      <c r="D2" s="19"/>
+      <c r="E2" s="9">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="str">
+      <c r="A3" s="11" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="12" t="str">
+      <c r="B3" s="11" t="str">
         <f>[1]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="12" t="str">
+      <c r="C3" s="11" t="str">
         <f>[1]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="12" t="str">
+      <c r="D3" s="11" t="str">
         <f>[1]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="10" t="str">
+      <c r="E3" s="9" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>14</v>
+      <c r="A9" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>29</v>
+      <c r="A10" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>25</v>
+      <c r="A11" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="D13" s="13"/>
       <c r="E13" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1079,417 +1081,421 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="19.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="str">
+      <c r="A1" s="16" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="19">
+      <c r="B1" s="18">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="19">
+      <c r="E1" s="18">
         <f>CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="19">
+      <c r="E2" s="18">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="str">
+      <c r="A3" s="16" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="17" t="str">
+      <c r="B3" s="16" t="str">
         <f>CONDUCTOR_files!B$3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="17" t="str">
+      <c r="C3" s="16" t="str">
         <f>CONDUCTOR_files!C$3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="17" t="str">
+      <c r="D3" s="16" t="str">
         <f>CONDUCTOR_files!D$3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="19" t="str">
+      <c r="E3" s="18" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>56</v>
+      <c r="A5" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>57</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>58</v>
+      <c r="A6" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>61</v>
+      <c r="A7" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>62</v>
+      <c r="A8" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>20</v>
+      <c r="A10" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>26</v>
+      <c r="A11" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="6">
+        <v>19</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="6">
+        <v>18</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>13</v>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>28</v>
+      <c r="A15" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>12</v>
+      <c r="A16" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="3">
-        <v>10001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="D18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="11" t="str">
+      <c r="E19" s="10" t="str">
         <f>E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+    <row r="20" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="E21" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="9">
+      <c r="E22" s="8">
         <v>0.5</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.5</v>
+      <c r="A24" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1517,130 +1523,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="str">
+      <c r="A1" s="31" t="str">
         <f>CONDUCTOR_files!A1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="32">
+      <c r="B1" s="31">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="33">
+      <c r="E1" s="32">
         <f>CONDUCTOR_files!E1</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <f>IF(E$1 &gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="str">
+      <c r="A3" s="31" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="32" t="str">
+      <c r="B3" s="31" t="str">
         <f>CONDUCTOR_files!B$3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="32" t="str">
+      <c r="C3" s="31" t="str">
         <f>CONDUCTOR_files!C$3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="32" t="str">
+      <c r="D3" s="31" t="str">
         <f>CONDUCTOR_files!D$3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="32" t="str">
+      <c r="E3" s="31" t="str">
         <f>CONDUCTOR_files!E3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="E6" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="34"/>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="D7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="39">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="35">
+      <c r="E8" s="34">
         <v>0</v>
       </c>
     </row>
@@ -1653,7 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -1664,18 +1670,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29" t="str">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="str">
+      <c r="A2" s="28" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: delete useless columns in sheet CONDUCTOR_operation.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB2B835-C2ED-4653-9C41-68DB766D52D5}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{058C9D53-254B-43B4-B3DB-9F85A94CAE5D}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -461,7 +461,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1465,36 +1464,36 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="36" t="s">
+      <c r="B23" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="35" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1507,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,13 +1521,13 @@
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="str">
         <f>CONDUCTOR_files!A1</f>
         <v>CONDUCTOR</v>
       </c>
       <c r="B1" s="31">
-        <f>SUM(E2:AE2)</f>
+        <f>SUM(E2:U2)</f>
         <v>1</v>
       </c>
       <c r="E1" s="32">
@@ -1536,13 +1535,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="32">
         <f>IF(E$1 &gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1564,8 +1563,8 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1580,10 +1579,9 @@
       <c r="E4" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="33"/>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1599,8 +1597,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1616,25 +1614,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="37">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1646,7 +1644,7 @@
       <c r="D8" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>0</v>
       </c>
     </row>

</xml_diff>